<commit_message>
eng question and herb img test
</commit_message>
<xml_diff>
--- a/test_questions_withANS.xlsx
+++ b/test_questions_withANS.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zirong/Desktop/CCD_RAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCE8557-9C1D-E340-8B72-CB5AB67A547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E8AF9B-CCCE-7E40-8864-64AA2C2952DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="860" windowWidth="25280" windowHeight="16960" xr2:uid="{49CF8178-EFA8-9643-BFB1-A8E39845DF37}"/>
+    <workbookView xWindow="7820" yWindow="-19540" windowWidth="25280" windowHeight="16960" xr2:uid="{49CF8178-EFA8-9643-BFB1-A8E39845DF37}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$I$120</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="294">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -502,10 +505,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RAG片段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>如果家犬出現焦躁、夜間吠叫，簡單按壓哪一穴可助安神？其大略位置為何？</t>
   </si>
   <si>
@@ -539,9 +538,6 @@
     <t>LI-4/LI-11/GV-14 清熱祛風；LU-5 清肺實熱，散肺止咳</t>
   </si>
   <si>
-    <t>LI-4, LI-11 and GV-14 are major points to disperse exterior and interior heat, while LU-5 (He-sea, water) clears Lung excess heat and stops coughing. :contentReference[oaicite:6]{index=6}&amp;#8203;:contentReference[oaicite:7]{index=7}</t>
-  </si>
-  <si>
     <t>肺氣虛犬常見臨床徵象及最重要的原穴是哪一個？</t>
   </si>
   <si>
@@ -608,9 +604,6 @@
     <t>DNMP 測驗主要評估聽覺記憶。</t>
   </si>
   <si>
-    <t>CCD 行為症狀常被飼主誤認為正常老化。</t>
-  </si>
-  <si>
     <t>DISHA 中的 H 代表 housesoiling。</t>
   </si>
   <si>
@@ -768,9 +761,6 @@
     <t>Recent evidence suggests the anticonvulsant drug levetiracetam improves cognitive function.</t>
   </si>
   <si>
-    <t>MRI 微出血檢出最佳序列為？ A) FLAIR B) T2* C) T1 加權 D) DWI</t>
-  </si>
-  <si>
     <t>T2*-weighted MRI sequences are useful in identifying haemorrhagic brain lesions in CCD.</t>
   </si>
   <si>
@@ -826,9 +816,6 @@
   </si>
   <si>
     <t>DISHA: … housesoiling is included.</t>
-  </si>
-  <si>
-    <t>CCD 患犬與末期 AD 人類同樣無法自行進食。</t>
   </si>
   <si>
     <t>Dogs do not show such extensive impairments; ability to eat is retained.</t>
@@ -967,10 +954,6 @@
   <si>
     <t>下列哪一穴位最常用來處理寵物的慢性咳嗽？
 A LU-1 中府 B LU-9 太淵 C LI-4 合谷</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>狗狗鼻塞流鼻水，建議在鼻翼外側 0.1 吋針刺的穴位是？A LI-20 B LI-11 C LU-7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1122,12 +1105,86 @@
       <t>Canine Cognitive Dysfunction Pathophysiology Diagnosis and Treatment.pdf</t>
     </r>
   </si>
+  <si>
+    <t>RAG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRI 微出血檢出最佳序列為？ A) FLAIR B) T2* C) T1 加權 D) DWI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCD 行為症狀常被飼主誤認為正常老化。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCD 患犬與末期 AD 人類同樣無法自行進食。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>狗狗鼻塞流鼻水，建議在鼻翼外側 0.1 吋針刺的穴位是？A LI-20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="蘋方-簡 標準體"/>
+        <charset val="134"/>
+      </rPr>
+      <t>B LI-11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="蘋方-簡 標準體"/>
+        <charset val="134"/>
+      </rPr>
+      <t>C LU-7</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiple_choice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI-4, LI-11 and GV-14 are major points to disperse exterior and interior heat, while LU-5 (He-sea, water) clears Lung excess heat and stops coughing. :contentReference[oaicite:6]{index=6}&amp;#8203;:contentReference[oaicite:7]{index=7}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1174,6 +1231,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1569,19 +1632,20 @@
   <dimension ref="A1:I173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="4" customWidth="1"/>
-    <col min="3" max="4" width="10.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="72.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="76" style="3" customWidth="1"/>
-    <col min="7" max="7" width="36" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="79.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="35.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -1608,10 +1672,10 @@
         <v>21</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>121</v>
+        <v>285</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="48" customHeight="1">
@@ -1640,7 +1704,7 @@
         <v>31</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="50">
@@ -1669,7 +1733,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="50">
@@ -1695,13 +1759,13 @@
         <v>15</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="50">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1727,10 +1791,10 @@
         <v>32</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="50">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1756,10 +1820,10 @@
         <v>33</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="50">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1785,10 +1849,10 @@
         <v>34</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="50">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1814,10 +1878,10 @@
         <v>35</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="50">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1843,10 +1907,10 @@
         <v>44</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="50">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1872,10 +1936,10 @@
         <v>45</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="50">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1898,10 +1962,10 @@
         <v>395</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="50">
@@ -1909,7 +1973,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>7</v>
@@ -1930,10 +1994,10 @@
         <v>46</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="50">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1959,7 +2023,7 @@
         <v>47</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="50">
@@ -1988,10 +2052,10 @@
         <v>48</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="50">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2017,7 +2081,7 @@
         <v>49</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="75">
@@ -2034,7 +2098,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>5</v>
@@ -2043,13 +2107,13 @@
         <v>560</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="50">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2075,10 +2139,10 @@
         <v>50</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="50">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2101,13 +2165,13 @@
         <v>14</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="50">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2133,10 +2197,10 @@
         <v>61</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="50">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2162,10 +2226,10 @@
         <v>62</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="50">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2191,7 +2255,7 @@
         <v>63</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="50">
@@ -2220,7 +2284,7 @@
         <v>64</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="50">
@@ -2249,7 +2313,7 @@
         <v>65</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="50">
@@ -2278,10 +2342,10 @@
         <v>66</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2307,10 +2371,10 @@
         <v>67</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="50">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2336,10 +2400,10 @@
         <v>68</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -2365,10 +2429,10 @@
         <v>69</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="50">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2394,10 +2458,10 @@
         <v>74</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="50">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2423,10 +2487,10 @@
         <v>75</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="50">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -2452,10 +2516,10 @@
         <v>76</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="75">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="50">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2478,10 +2542,10 @@
         <v>75</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="50">
@@ -2510,7 +2574,7 @@
         <v>93</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="50">
@@ -2539,7 +2603,7 @@
         <v>92</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="50">
@@ -2568,7 +2632,7 @@
         <v>91</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="50">
@@ -2597,7 +2661,7 @@
         <v>90</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="50">
@@ -2626,7 +2690,7 @@
         <v>89</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="50">
@@ -2655,7 +2719,7 @@
         <v>88</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="75">
@@ -2681,10 +2745,10 @@
         <v>21</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="50">
@@ -2713,7 +2777,7 @@
         <v>87</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="50">
@@ -2742,7 +2806,7 @@
         <v>86</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="50">
@@ -2771,7 +2835,7 @@
         <v>105</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="50">
@@ -2800,7 +2864,7 @@
         <v>104</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="50">
@@ -2829,7 +2893,7 @@
         <v>103</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="50">
@@ -2858,7 +2922,7 @@
         <v>102</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="50">
@@ -2887,7 +2951,7 @@
         <v>101</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="50">
@@ -2916,10 +2980,10 @@
         <v>100</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="50">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2933,7 +2997,7 @@
         <v>9</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>5</v>
@@ -2945,10 +3009,10 @@
         <v>107</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="50">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -2962,7 +3026,7 @@
         <v>9</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>10</v>
@@ -2974,10 +3038,10 @@
         <v>108</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="50">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -2991,7 +3055,7 @@
         <v>9</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>5</v>
@@ -3003,10 +3067,10 @@
         <v>109</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="50">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -3020,7 +3084,7 @@
         <v>9</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>4</v>
@@ -3032,10 +3096,10 @@
         <v>113</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="50">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -3049,7 +3113,7 @@
         <v>9</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>10</v>
@@ -3061,10 +3125,10 @@
         <v>112</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="50">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -3078,7 +3142,7 @@
         <v>9</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>4</v>
@@ -3090,10 +3154,10 @@
         <v>110</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="50">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -3107,7 +3171,7 @@
         <v>9</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>10</v>
@@ -3119,10 +3183,10 @@
         <v>111</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="75">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="50">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -3136,7 +3200,7 @@
         <v>9</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>5</v>
@@ -3148,7 +3212,7 @@
         <v>110</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="100">
@@ -3165,7 +3229,7 @@
         <v>9</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>5</v>
@@ -3177,7 +3241,7 @@
         <v>114</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="75">
@@ -3194,7 +3258,7 @@
         <v>9</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>10</v>
@@ -3206,7 +3270,7 @@
         <v>115</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="75">
@@ -3223,7 +3287,7 @@
         <v>9</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>4</v>
@@ -3235,10 +3299,10 @@
         <v>116</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="50">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -3252,7 +3316,7 @@
         <v>9</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>4</v>
@@ -3264,10 +3328,10 @@
         <v>117</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="50">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -3281,7 +3345,7 @@
         <v>9</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>10</v>
@@ -3293,10 +3357,10 @@
         <v>118</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="75">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="50">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -3310,7 +3374,7 @@
         <v>9</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>5</v>
@@ -3322,7 +3386,7 @@
         <v>119</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="100">
@@ -3339,7 +3403,7 @@
         <v>9</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>10</v>
@@ -3351,7 +3415,7 @@
         <v>120</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="125">
@@ -3368,19 +3432,19 @@
         <v>9</v>
       </c>
       <c r="E62" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="G62" s="7">
         <v>36</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="125">
@@ -3397,19 +3461,19 @@
         <v>9</v>
       </c>
       <c r="E63" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F63" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="F63" s="6" t="s">
+      <c r="G63" s="7">
+        <v>9</v>
+      </c>
+      <c r="H63" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G63" s="7">
-        <v>9</v>
-      </c>
-      <c r="H63" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="I63" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="125">
@@ -3426,19 +3490,19 @@
         <v>9</v>
       </c>
       <c r="E64" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F64" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>129</v>
       </c>
       <c r="G64" s="7">
         <v>15</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="125">
@@ -3455,19 +3519,19 @@
         <v>9</v>
       </c>
       <c r="E65" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F65" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>132</v>
       </c>
       <c r="G65" s="7">
         <v>285</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>133</v>
+        <v>293</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="125">
@@ -3484,19 +3548,19 @@
         <v>9</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G66" s="7">
         <v>153</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="75">
@@ -3513,19 +3577,19 @@
         <v>9</v>
       </c>
       <c r="E67" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G67" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="F67" s="6" t="s">
+      <c r="H67" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G67" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>140</v>
-      </c>
       <c r="I67" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="125">
@@ -3542,19 +3606,19 @@
         <v>9</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G68" s="7">
         <v>52</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="100">
@@ -3571,19 +3635,19 @@
         <v>9</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G69" s="7">
         <v>3</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="125">
@@ -3600,19 +3664,19 @@
         <v>9</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G70" s="7">
         <v>285</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="150">
@@ -3623,25 +3687,25 @@
         <v>20</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>6</v>
+        <v>292</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G71" s="7">
         <v>241</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="100">
@@ -3652,11 +3716,13 @@
         <v>20</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="7"/>
+        <v>291</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E72" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>13</v>
@@ -3665,10 +3731,10 @@
         <v>6</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="100">
@@ -3679,11 +3745,13 @@
         <v>20</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D73" s="7"/>
+        <v>291</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E73" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>16</v>
@@ -3692,13 +3760,13 @@
         <v>6</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="75">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="50">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -3706,11 +3774,13 @@
         <v>20</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" s="7"/>
+        <v>291</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E74" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>15</v>
@@ -3719,13 +3789,13 @@
         <v>2</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="75">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="50">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -3735,9 +3805,11 @@
       <c r="C75" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="7"/>
+      <c r="D75" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E75" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>15</v>
@@ -3746,13 +3818,13 @@
         <v>2</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="100">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="75">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -3762,9 +3834,11 @@
       <c r="C76" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D76" s="7"/>
+      <c r="D76" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E76" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>15</v>
@@ -3773,13 +3847,13 @@
         <v>8</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I76" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="75">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -3789,9 +3863,11 @@
       <c r="C77" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="7"/>
+      <c r="D77" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E77" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>15</v>
@@ -3800,13 +3876,13 @@
         <v>11</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I77" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="75">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -3816,9 +3892,11 @@
       <c r="C78" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D78" s="7"/>
+      <c r="D78" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E78" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>14</v>
@@ -3827,13 +3905,13 @@
         <v>7</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="75">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -3843,9 +3921,11 @@
       <c r="C79" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D79" s="7"/>
+      <c r="D79" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E79" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>15</v>
@@ -3854,13 +3934,13 @@
         <v>12</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I79" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="75">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -3870,9 +3950,11 @@
       <c r="C80" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D80" s="7"/>
+      <c r="D80" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E80" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>14</v>
@@ -3881,13 +3963,13 @@
         <v>13</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="75">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -3897,9 +3979,11 @@
       <c r="C81" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D81" s="7"/>
+      <c r="D81" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E81" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>16</v>
@@ -3908,13 +3992,13 @@
         <v>13</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I81" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="75">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -3924,9 +4008,11 @@
       <c r="C82" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D82" s="7"/>
+      <c r="D82" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E82" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>15</v>
@@ -3935,13 +4021,13 @@
         <v>7</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I82" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="75">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -3951,9 +4037,11 @@
       <c r="C83" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="7"/>
+      <c r="D83" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E83" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>15</v>
@@ -3962,13 +4050,13 @@
         <v>12</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="75">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -3978,9 +4066,11 @@
       <c r="C84" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D84" s="7"/>
+      <c r="D84" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E84" s="7" t="s">
-        <v>209</v>
+        <v>286</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>15</v>
@@ -3989,13 +4079,13 @@
         <v>8</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="75">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="50">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -4005,9 +4095,11 @@
       <c r="C85" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="7"/>
+      <c r="D85" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E85" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>14</v>
@@ -4016,10 +4108,10 @@
         <v>3</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I85" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="75">
@@ -4032,9 +4124,11 @@
       <c r="C86" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D86" s="7"/>
+      <c r="D86" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E86" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>14</v>
@@ -4043,13 +4137,13 @@
         <v>3</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I86" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="75">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="50">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -4059,9 +4153,11 @@
       <c r="C87" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D87" s="7"/>
+      <c r="D87" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E87" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>13</v>
@@ -4070,13 +4166,13 @@
         <v>3</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="75">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="50">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -4086,9 +4182,11 @@
       <c r="C88" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D88" s="7"/>
+      <c r="D88" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E88" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>16</v>
@@ -4097,13 +4195,13 @@
         <v>4</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I88" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="100">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="75">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -4113,9 +4211,11 @@
       <c r="C89" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D89" s="7"/>
+      <c r="D89" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E89" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>15</v>
@@ -4124,13 +4224,13 @@
         <v>13</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I89" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="75">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="50">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -4140,9 +4240,11 @@
       <c r="C90" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D90" s="7"/>
+      <c r="D90" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E90" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>13</v>
@@ -4151,13 +4253,13 @@
         <v>3</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I90" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="75">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="50">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -4167,9 +4269,11 @@
       <c r="C91" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D91" s="7"/>
+      <c r="D91" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E91" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>14</v>
@@ -4178,10 +4282,10 @@
         <v>4</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I91" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="100">
@@ -4194,9 +4298,11 @@
       <c r="C92" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D92" s="7"/>
+      <c r="D92" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E92" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F92" s="6" t="b">
         <v>1</v>
@@ -4205,13 +4311,13 @@
         <v>6</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I92" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="100">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="75">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -4221,9 +4327,11 @@
       <c r="C93" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D93" s="7"/>
+      <c r="D93" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E93" s="7" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F93" s="6" t="b">
         <v>0</v>
@@ -4232,13 +4340,13 @@
         <v>8</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="75">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -4248,9 +4356,11 @@
       <c r="C94" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D94" s="7"/>
+      <c r="D94" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E94" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F94" s="6" t="b">
         <v>0</v>
@@ -4259,13 +4369,13 @@
         <v>11</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="75">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -4275,9 +4385,11 @@
       <c r="C95" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D95" s="7"/>
+      <c r="D95" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E95" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F95" s="6" t="b">
         <v>0</v>
@@ -4286,10 +4398,10 @@
         <v>7</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I95" s="7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="50">
@@ -4302,9 +4414,11 @@
       <c r="C96" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D96" s="7"/>
+      <c r="D96" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E96" s="7" t="s">
-        <v>156</v>
+        <v>287</v>
       </c>
       <c r="F96" s="6" t="b">
         <v>1</v>
@@ -4313,10 +4427,10 @@
         <v>3</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I96" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="100">
@@ -4329,9 +4443,11 @@
       <c r="C97" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D97" s="7"/>
+      <c r="D97" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E97" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F97" s="6" t="b">
         <v>1</v>
@@ -4340,10 +4456,10 @@
         <v>6</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I97" s="7" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="100">
@@ -4356,9 +4472,11 @@
       <c r="C98" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D98" s="7"/>
+      <c r="D98" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E98" s="7" t="s">
-        <v>229</v>
+        <v>288</v>
       </c>
       <c r="F98" s="6" t="b">
         <v>0</v>
@@ -4367,13 +4485,13 @@
         <v>6</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I98" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="100">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="75">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -4383,9 +4501,11 @@
       <c r="C99" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D99" s="7"/>
+      <c r="D99" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E99" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F99" s="6" t="b">
         <v>1</v>
@@ -4394,10 +4514,10 @@
         <v>13</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I99" s="7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="50">
@@ -4410,9 +4530,11 @@
       <c r="C100" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D100" s="7"/>
+      <c r="D100" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E100" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F100" s="6" t="b">
         <v>1</v>
@@ -4421,10 +4543,10 @@
         <v>3</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I100" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="19" customHeight="1">
@@ -4437,9 +4559,11 @@
       <c r="C101" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D101" s="7"/>
+      <c r="D101" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E101" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F101" s="6" t="b">
         <v>0</v>
@@ -4448,13 +4572,13 @@
         <v>12</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I101" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="75">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -4464,9 +4588,11 @@
       <c r="C102" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D102" s="7"/>
+      <c r="D102" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E102" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F102" s="6" t="b">
         <v>1</v>
@@ -4475,13 +4601,13 @@
         <v>8</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I102" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="75">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -4491,9 +4617,11 @@
       <c r="C103" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D103" s="7"/>
+      <c r="D103" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E103" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F103" s="6" t="b">
         <v>1</v>
@@ -4502,13 +4630,13 @@
         <v>8</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I103" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="75">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -4518,9 +4646,11 @@
       <c r="C104" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D104" s="7"/>
+      <c r="D104" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E104" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F104" s="6" t="b">
         <v>1</v>
@@ -4529,13 +4659,13 @@
         <v>8</v>
       </c>
       <c r="H104" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="75">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -4545,9 +4675,11 @@
       <c r="C105" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D105" s="7"/>
+      <c r="D105" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E105" s="7" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F105" s="6" t="b">
         <v>1</v>
@@ -4556,13 +4688,13 @@
         <v>12</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I105" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="75">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -4572,9 +4704,11 @@
       <c r="C106" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D106" s="7"/>
+      <c r="D106" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E106" s="7" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F106" s="6" t="b">
         <v>1</v>
@@ -4583,13 +4717,13 @@
         <v>13</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="I106" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="75">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -4599,9 +4733,11 @@
       <c r="C107" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D107" s="7"/>
+      <c r="D107" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E107" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F107" s="6" t="b">
         <v>0</v>
@@ -4610,10 +4746,10 @@
         <v>12</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="I107" s="7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="50">
@@ -4626,9 +4762,11 @@
       <c r="C108" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D108" s="7"/>
+      <c r="D108" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E108" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F108" s="6" t="b">
         <v>1</v>
@@ -4637,10 +4775,10 @@
         <v>4</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="I108" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="50">
@@ -4653,9 +4791,11 @@
       <c r="C109" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D109" s="7"/>
+      <c r="D109" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E109" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F109" s="6" t="b">
         <v>0</v>
@@ -4664,10 +4804,10 @@
         <v>3</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I109" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="50">
@@ -4680,9 +4820,11 @@
       <c r="C110" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D110" s="7"/>
+      <c r="D110" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E110" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F110" s="6" t="b">
         <v>0</v>
@@ -4691,13 +4833,13 @@
         <v>3</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I110" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" ht="100">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="75">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -4707,21 +4849,23 @@
       <c r="C111" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D111" s="7"/>
+      <c r="D111" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E111" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G111" s="7">
         <v>8</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I111" s="7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="100">
@@ -4734,24 +4878,26 @@
       <c r="C112" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D112" s="7"/>
+      <c r="D112" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E112" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G112" s="7">
         <v>6</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="I112" s="7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="100">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="75">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -4761,24 +4907,26 @@
       <c r="C113" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D113" s="7"/>
+      <c r="D113" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E113" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G113" s="7">
         <v>11</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="75">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -4788,21 +4936,23 @@
       <c r="C114" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D114" s="7"/>
+      <c r="D114" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E114" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G114" s="7">
         <v>7</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="I114" s="7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="50">
@@ -4815,24 +4965,26 @@
       <c r="C115" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="7"/>
+      <c r="D115" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E115" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G115" s="7">
         <v>3</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" ht="100">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="75">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -4842,24 +4994,26 @@
       <c r="C116" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="7"/>
+      <c r="D116" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E116" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G116" s="7">
         <v>13</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="I116" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="75">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -4869,24 +5023,26 @@
       <c r="C117" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D117" s="7"/>
+      <c r="D117" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E117" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="G117" s="7">
         <v>8</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="I117" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" ht="100">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="75">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -4896,21 +5052,23 @@
       <c r="C118" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D118" s="7"/>
+      <c r="D118" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E118" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G118" s="7">
         <v>12</v>
       </c>
       <c r="H118" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="I118" s="7" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="50">
@@ -4923,21 +5081,23 @@
       <c r="C119" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D119" s="7"/>
+      <c r="D119" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E119" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G119" s="7">
         <v>2</v>
       </c>
       <c r="H119" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="I119" s="7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="100">
@@ -4950,21 +5110,23 @@
       <c r="C120" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D120" s="7"/>
+      <c r="D120" s="7" t="s">
+        <v>290</v>
+      </c>
       <c r="E120" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G120" s="7">
         <v>6</v>
       </c>
       <c r="H120" s="7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I120" s="7" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -5127,6 +5289,7 @@
       <c r="A173" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I120" xr:uid="{E27A6E25-28F7-6A43-9063-8BB9C579CCE6}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>